<commit_message>
fixed outlier removal, added data collection templates
</commit_message>
<xml_diff>
--- a/tests/eugl_1.xlsx
+++ b/tests/eugl_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanallen\Desktop\spectral_pv_curves\spectral_pv_curves\data\eugl_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanallen\Desktop\pvtools\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF601D1-437C-424F-A229-D7795A4D485B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AD78E9-2955-4680-8B6F-AFD02D94CF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15435" xr2:uid="{CCE13063-7B56-4144-BB29-38D08D7031CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CCE13063-7B56-4144-BB29-38D08D7031CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -56,15 +59,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Time</t>
   </si>
   <si>
     <t>Y (Mpa)</t>
-  </si>
-  <si>
-    <t>(-1/Y)</t>
   </si>
   <si>
     <t>Mass (g)</t>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>Dry Weight (g)</t>
-  </si>
-  <si>
-    <t>Leaf Thickness (mm)</t>
   </si>
   <si>
     <t>RWC</t>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>(1/Y)</t>
   </si>
 </sst>
 </file>
@@ -405,10 +405,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$20</c:f>
+              <c:f>Sheet1!$F$2:$F$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -465,72 +465,126 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>4.6424408291520933</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.2252800162181359</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.853732704880656</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.5582078962039532</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.176524251178364</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.7121788049262534</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10.080583852820439</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$20</c:f>
+              <c:f>Sheet1!$C$2:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5087719298245617</c:v>
+                  <c:v>-3.5087719298245617</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3222591362126246</c:v>
+                  <c:v>-3.3222591362126246</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7777777777777777</c:v>
+                  <c:v>-2.7777777777777777</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.3255813953488373</c:v>
+                  <c:v>-2.3255813953488373</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0833333333333335</c:v>
+                  <c:v>-2.0833333333333335</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8181818181818181</c:v>
+                  <c:v>-1.8181818181818181</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.5384615384615383</c:v>
+                  <c:v>-1.5384615384615383</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2853470437017995</c:v>
+                  <c:v>-1.2853470437017995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0309278350515465</c:v>
+                  <c:v>-1.0309278350515465</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.8857395925597874</c:v>
+                  <c:v>-0.8857395925597874</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.77639751552795033</c:v>
+                  <c:v>-0.77639751552795033</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.67796610169491522</c:v>
+                  <c:v>-0.67796610169491522</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.63694267515923564</c:v>
+                  <c:v>-0.63694267515923564</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.6097560975609756</c:v>
+                  <c:v>-0.6097560975609756</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.59594755661501786</c:v>
+                  <c:v>-0.59594755661501786</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.56818181818181823</c:v>
+                  <c:v>-0.56818181818181823</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.52137643378519294</c:v>
+                  <c:v>-0.52137643378519294</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.50251256281407031</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.48309178743961356</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.47619047619047616</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.46082949308755761</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.43103448275862072</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.41152263374485593</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -543,10 +597,18 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Trendline</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$M$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Preliminary Turgor Loss Point Curve</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -556,19 +618,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:trendline>
             <c:spPr>
-              <a:ln w="12700" cap="rnd">
+              <a:ln w="19050" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="tx2"/>
                 </a:solidFill>
@@ -577,57 +631,16 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="1"/>
-            <c:backward val="2"/>
-            <c:dispRSqr val="1"/>
+            <c:backward val="7"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="4.1417408189829932E-2"/>
-                  <c:y val="-0.56184231976962218"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-                <a:ln>
-                  <a:solidFill>
-                    <a:schemeClr val="bg2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$N$9:$N$12</c:f>
+              <c:f>Sheet1!$N$9:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>5.853732704880656</c:v>
                 </c:pt>
@@ -639,27 +652,33 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8.7121788049262534</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.080583852820439</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$M$9:$M$12</c:f>
+              <c:f>Sheet1!$M$9:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.48309178743961356</c:v>
+                  <c:v>-0.48309178743961356</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.47619047619047616</c:v>
+                  <c:v>-0.47619047619047616</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.46082949308755761</c:v>
+                  <c:v>-0.46082949308755761</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.43103448275862072</c:v>
+                  <c:v>-0.43103448275862072</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.41152263374485593</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -667,7 +686,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2B5E-4D3D-ACE0-B0D0720A57A9}"/>
+              <c16:uniqueId val="{00000002-8F7E-406C-84F9-EA0DEA2BEF86}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -686,6 +705,7 @@
         <c:axId val="1192320895"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1862,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11C6E8C-53E4-4B63-89A1-4561B5D848E3}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,7 +1894,7 @@
     <col min="11" max="12" width="5.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1882,52 +1902,49 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="M1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="O1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>45317.33865636574</v>
       </c>
       <c r="B2" s="10">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="C2" s="1">
         <f>1/B2</f>
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="D2" s="10">
         <v>1.9731000000000001</v>
@@ -1941,7 +1958,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1">
-        <f>(D2-$O$2)/($D$2-$O$2)</f>
+        <f t="shared" ref="G2:G29" si="1">(D2-$N$2)/($D$2-$N$2)</f>
         <v>1</v>
       </c>
       <c r="H2" s="10">
@@ -1952,30 +1969,29 @@
         <v>20240126_00000</v>
       </c>
       <c r="J2" s="1">
-        <f>(D2-$O$2)/$P$2</f>
+        <f>(D2-$N$2)/$O$2</f>
         <v>2.8108569750994152E-2</v>
       </c>
       <c r="M2" s="11">
         <v>45317</v>
       </c>
-      <c r="N2" s="10"/>
+      <c r="N2" s="10">
+        <v>0.91990000000000005</v>
+      </c>
       <c r="O2" s="10">
-        <v>0.91990000000000005</v>
-      </c>
-      <c r="P2" s="10">
         <v>37.469000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>45317.339988541666</v>
       </c>
       <c r="B3" s="10">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C29" si="1">1/B3</f>
-        <v>4</v>
+        <f t="shared" ref="C3:C29" si="2">1/B3</f>
+        <v>-4</v>
       </c>
       <c r="D3" s="10">
         <v>1.9704999999999999</v>
@@ -1985,11 +2001,11 @@
         <v>99.868227662054622</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F20" si="2">IF(E3=0,NA(),100-E3)</f>
+        <f t="shared" ref="F3:F20" si="3">IF(E3=0,NA(),100-E3)</f>
         <v>0.13177233794537813</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G20" si="3">(D3-$O$2)/($D$2-$O$2)</f>
+        <f t="shared" si="1"/>
         <v>0.99753133308013653</v>
       </c>
       <c r="H3" s="10">
@@ -2000,20 +2016,20 @@
         <v>20240126_00001</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" ref="J3:J20" si="5">(D3-$O$2)/$P$2</f>
+        <f t="shared" ref="J3:J20" si="5">(D3-$N$2)/$O$2</f>
         <v>2.8039179054685198E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>45317.340970138888</v>
       </c>
       <c r="B4" s="10">
-        <v>0.28499999999999998</v>
+        <v>-0.28499999999999998</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="1"/>
-        <v>3.5087719298245617</v>
+        <f t="shared" si="2"/>
+        <v>-3.5087719298245617</v>
       </c>
       <c r="D4" s="10">
         <v>1.9688000000000001</v>
@@ -2023,11 +2039,11 @@
         <v>99.78206882570575</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.21793117429425024</v>
       </c>
       <c r="G4" s="1">
-        <f>(D4-$O$2)/($D$2-$O$2)</f>
+        <f t="shared" si="1"/>
         <v>0.9959172047094571</v>
       </c>
       <c r="H4" s="10">
@@ -2042,16 +2058,16 @@
         <v>2.7993808214790899E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>45317.34208263889</v>
       </c>
       <c r="B5" s="10">
-        <v>0.30099999999999999</v>
+        <v>-0.30099999999999999</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="1"/>
-        <v>3.3222591362126246</v>
+        <f t="shared" si="2"/>
+        <v>-3.3222591362126246</v>
       </c>
       <c r="D5" s="10">
         <v>1.9670000000000001</v>
@@ -2061,11 +2077,11 @@
         <v>99.690841822512809</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.30915817748719121</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.99420812761109001</v>
       </c>
       <c r="H5" s="10">
@@ -2080,16 +2096,16 @@
         <v>2.7945768501961617E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>45317.343275231484</v>
       </c>
       <c r="B6" s="10">
-        <v>0.36</v>
+        <v>-0.36</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="1"/>
-        <v>2.7777777777777777</v>
+        <f t="shared" si="2"/>
+        <v>-2.7777777777777777</v>
       </c>
       <c r="D6" s="10">
         <v>1.9646999999999999</v>
@@ -2099,11 +2115,11 @@
         <v>99.57427398509958</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.42572601490041961</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.99202430687428789</v>
       </c>
       <c r="H6" s="10">
@@ -2114,20 +2130,20 @@
         <v>20240126_00004</v>
       </c>
       <c r="J6" s="1">
-        <f>(D6-$O$2)/$P$2</f>
+        <f>(D6-$N$2)/$O$2</f>
         <v>2.7884384424457551E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>45317.344400231479</v>
       </c>
       <c r="B7" s="10">
-        <v>0.43</v>
+        <v>-0.43</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="1"/>
-        <v>2.3255813953488373</v>
+        <f t="shared" si="2"/>
+        <v>-2.3255813953488373</v>
       </c>
       <c r="D7" s="10">
         <v>1.9623999999999999</v>
@@ -2137,11 +2153,11 @@
         <v>99.457706147686366</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.54229385231363381</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.98984048613748588</v>
       </c>
       <c r="H7" s="10">
@@ -2156,20 +2172,20 @@
         <v>2.782300034695348E-2</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>45317.34549803241</v>
       </c>
       <c r="B8" s="10">
-        <v>0.48</v>
+        <v>-0.48</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333335</v>
+        <f t="shared" si="2"/>
+        <v>-2.0833333333333335</v>
       </c>
       <c r="D8" s="10">
         <v>1.9595</v>
@@ -2179,11 +2195,11 @@
         <v>99.310729309208853</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.68927069079114744</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.9870869730345615</v>
       </c>
       <c r="H8" s="10">
@@ -2198,22 +2214,22 @@
         <v>2.7745603031839657E-2</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>45317.346652199078</v>
       </c>
       <c r="B9" s="10">
-        <v>0.55000000000000004</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="1"/>
-        <v>1.8181818181818181</v>
+        <f t="shared" si="2"/>
+        <v>-1.8181818181818181</v>
       </c>
       <c r="D9" s="10">
         <v>1.9560999999999999</v>
@@ -2223,11 +2239,11 @@
         <v>99.138411636511066</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.86158836348893431</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.98385871629320176</v>
       </c>
       <c r="H9" s="10">
@@ -2243,23 +2259,23 @@
       </c>
       <c r="M9" s="1" cm="1">
         <f t="array" aca="1" ref="M9:M13" ca="1">OFFSET(C1,COUNT(C:C),0,-5)</f>
-        <v>0.48309178743961356</v>
+        <v>-0.48309178743961356</v>
       </c>
       <c r="N9" s="1" cm="1">
         <f t="array" aca="1" ref="N9:N13" ca="1">OFFSET(F1,COUNT(F:F),0,-5)</f>
         <v>5.853732704880656</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>45317.34788321759</v>
       </c>
       <c r="B10" s="10">
-        <v>0.65</v>
+        <v>-0.65</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="1"/>
-        <v>1.5384615384615383</v>
+        <f t="shared" si="2"/>
+        <v>-1.5384615384615383</v>
       </c>
       <c r="D10" s="10">
         <v>1.9521999999999999</v>
@@ -2269,11 +2285,11 @@
         <v>98.94075312959302</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0592468704069802</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.98015571591340667</v>
       </c>
       <c r="H10" s="10">
@@ -2289,23 +2305,23 @@
       </c>
       <c r="M10" s="1">
         <f ca="1"/>
-        <v>0.47619047619047616</v>
+        <v>-0.47619047619047616</v>
       </c>
       <c r="N10" s="1">
         <f ca="1"/>
         <v>6.5582078962039532</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>45317.349226736114</v>
       </c>
       <c r="B11" s="10">
-        <v>0.77800000000000002</v>
+        <v>-0.77800000000000002</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="1"/>
-        <v>1.2853470437017995</v>
+        <f t="shared" si="2"/>
+        <v>-1.2853470437017995</v>
       </c>
       <c r="D11" s="10">
         <v>1.9466000000000001</v>
@@ -2315,11 +2331,11 @@
         <v>98.656935786326102</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3430642136738982</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.97483858716293204</v>
       </c>
       <c r="H11" s="10">
@@ -2335,23 +2351,23 @@
       </c>
       <c r="M11" s="1">
         <f ca="1"/>
-        <v>0.46082949308755761</v>
+        <v>-0.46082949308755761</v>
       </c>
       <c r="N11" s="1">
         <f ca="1"/>
         <v>7.176524251178364</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>45317.351053009261</v>
       </c>
       <c r="B12" s="10">
-        <v>0.97</v>
+        <v>-0.97</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="1"/>
-        <v>1.0309278350515465</v>
+        <f t="shared" si="2"/>
+        <v>-1.0309278350515465</v>
       </c>
       <c r="D12" s="10">
         <v>1.9391</v>
@@ -2361,11 +2377,11 @@
         <v>98.276823273022146</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.7231767269778544</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.96771743258640353</v>
       </c>
       <c r="H12" s="10">
@@ -2381,23 +2397,23 @@
       </c>
       <c r="M12" s="1">
         <f ca="1"/>
-        <v>0.43103448275862072</v>
+        <v>-0.43103448275862072</v>
       </c>
       <c r="N12" s="1">
         <f ca="1"/>
         <v>8.7121788049262534</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>45317.352708449071</v>
       </c>
       <c r="B13" s="10">
-        <v>1.129</v>
+        <v>-1.129</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="1"/>
-        <v>0.8857395925597874</v>
+        <f t="shared" si="2"/>
+        <v>-0.8857395925597874</v>
       </c>
       <c r="D13" s="10">
         <v>1.9318</v>
@@ -2407,11 +2423,11 @@
         <v>97.906847093406313</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.0931529065936871</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.96078617546524869</v>
       </c>
       <c r="H13" s="10">
@@ -2427,23 +2443,23 @@
       </c>
       <c r="M13" s="1">
         <f ca="1"/>
-        <v>0.41152263374485593</v>
+        <v>-0.41152263374485593</v>
       </c>
       <c r="N13" s="1">
         <f ca="1"/>
         <v>10.080583852820439</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>45317.354247916664</v>
       </c>
       <c r="B14" s="10">
-        <v>1.288</v>
+        <v>-1.288</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="1"/>
-        <v>0.77639751552795033</v>
+        <f t="shared" si="2"/>
+        <v>-0.77639751552795033</v>
       </c>
       <c r="D14" s="10">
         <v>1.9246000000000001</v>
@@ -2453,11 +2469,11 @@
         <v>97.541939080634535</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.4580609193654652</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.95394986707178142</v>
       </c>
       <c r="H14" s="10">
@@ -2472,16 +2488,16 @@
         <v>2.6814166377538768E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>45317.356958912038</v>
       </c>
       <c r="B15" s="10">
-        <v>1.4750000000000001</v>
+        <v>-1.4750000000000001</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="1"/>
-        <v>0.67796610169491522</v>
+        <f t="shared" si="2"/>
+        <v>-0.67796610169491522</v>
       </c>
       <c r="D15" s="10">
         <v>1.9152</v>
@@ -2491,11 +2507,11 @@
         <v>97.065531397293597</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.9344686027064029</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.9450246866691987</v>
       </c>
       <c r="H15" s="10">
@@ -2510,16 +2526,16 @@
         <v>2.6563292321652564E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>45317.358479513889</v>
       </c>
       <c r="B16" s="10">
-        <v>1.57</v>
+        <v>-1.57</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="1"/>
-        <v>0.63694267515923564</v>
+        <f t="shared" si="2"/>
+        <v>-0.63694267515923564</v>
       </c>
       <c r="D16" s="10">
         <v>1.9108000000000001</v>
@@ -2529,11 +2545,11 @@
         <v>96.842532056155292</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.1574679438447077</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.94084694265096858</v>
       </c>
       <c r="H16" s="10">
@@ -2553,11 +2569,11 @@
         <v>45317.360966898152</v>
       </c>
       <c r="B17" s="10">
-        <v>1.64</v>
+        <v>-1.64</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="1"/>
-        <v>0.6097560975609756</v>
+        <f t="shared" si="2"/>
+        <v>-0.6097560975609756</v>
       </c>
       <c r="D17" s="10">
         <v>1.9061999999999999</v>
@@ -2567,11 +2583,11 @@
         <v>96.609396381328864</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.3906036186711361</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.93647930117736411</v>
       </c>
       <c r="H17" s="10">
@@ -2591,11 +2607,11 @@
         <v>45317.364608912038</v>
       </c>
       <c r="B18" s="10">
-        <v>1.6779999999999999</v>
+        <v>-1.6779999999999999</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="1"/>
-        <v>0.59594755661501786</v>
+        <f t="shared" si="2"/>
+        <v>-0.59594755661501786</v>
       </c>
       <c r="D18" s="10">
         <v>1.9017999999999999</v>
@@ -2605,11 +2621,11 @@
         <v>96.386397040190559</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.613602959809441</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.93230155715913399</v>
       </c>
       <c r="H18" s="10">
@@ -2629,11 +2645,11 @@
         <v>45317.373170486113</v>
       </c>
       <c r="B19" s="10">
-        <v>1.76</v>
+        <v>-1.76</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="1"/>
-        <v>0.56818181818181823</v>
+        <f t="shared" si="2"/>
+        <v>-0.56818181818181823</v>
       </c>
       <c r="D19" s="10">
         <v>1.8927</v>
@@ -2643,11 +2659,11 @@
         <v>95.925193857381785</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.0748061426182147</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.92366122293961272</v>
       </c>
       <c r="H19" s="10">
@@ -2667,11 +2683,11 @@
         <v>45317.385397337966</v>
       </c>
       <c r="B20" s="10">
-        <v>1.9179999999999999</v>
+        <v>-1.9179999999999999</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="1"/>
-        <v>0.52137643378519294</v>
+        <f t="shared" si="2"/>
+        <v>-0.52137643378519294</v>
       </c>
       <c r="D20" s="10">
         <v>1.8815</v>
@@ -2681,11 +2697,11 @@
         <v>95.357559170847907</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.6424408291520933</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.91302696543866313</v>
       </c>
       <c r="H20" s="10">
@@ -2705,11 +2721,11 @@
         <v>45317.401966087964</v>
       </c>
       <c r="B21" s="10">
-        <v>1.99</v>
+        <v>-1.99</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="1"/>
-        <v>0.50251256281407031</v>
+        <f t="shared" si="2"/>
+        <v>-0.50251256281407031</v>
       </c>
       <c r="D21" s="10">
         <v>1.87</v>
@@ -2723,18 +2739,18 @@
         <v>5.2252800162181359</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" ref="G21:G29" si="9">(D21-$O$2)/($D$2-$O$2)</f>
+        <f t="shared" si="1"/>
         <v>0.90210786175465263</v>
       </c>
       <c r="H21" s="10">
         <v>39</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f t="shared" ref="I21:I29" si="10">_xlfn.CONCAT(TEXT($M$2,"yyyymmdd"),"_",TEXT(H21,"00000"))</f>
+        <f t="shared" ref="I21:I29" si="9">_xlfn.CONCAT(TEXT($M$2,"yyyymmdd"),"_",TEXT(H21,"00000"))</f>
         <v>20240126_00039</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" ref="J21:J29" si="11">(D21-$O$2)/$P$2</f>
+        <f t="shared" ref="J21:J29" si="10">(D21-$N$2)/$O$2</f>
         <v>2.5356961755050842E-2</v>
       </c>
     </row>
@@ -2743,11 +2759,11 @@
         <v>45317.425820254626</v>
       </c>
       <c r="B22" s="10">
-        <v>2.0699999999999998</v>
+        <v>-2.0699999999999998</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="1"/>
-        <v>0.48309178743961356</v>
+        <f t="shared" si="2"/>
+        <v>-0.48309178743961356</v>
       </c>
       <c r="D22" s="10">
         <v>1.8575999999999999</v>
@@ -2761,18 +2777,18 @@
         <v>5.853732704880656</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.89033421952145841</v>
       </c>
       <c r="H22" s="10">
         <v>48</v>
       </c>
       <c r="I22" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>20240126_00048</v>
+      </c>
+      <c r="J22" s="1">
         <f t="shared" si="10"/>
-        <v>20240126_00048</v>
-      </c>
-      <c r="J22" s="1">
-        <f t="shared" si="11"/>
         <v>2.502602151111585E-2</v>
       </c>
     </row>
@@ -2781,11 +2797,11 @@
         <v>45317.452658796297</v>
       </c>
       <c r="B23" s="10">
-        <v>2.1</v>
+        <v>-2.1</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="1"/>
-        <v>0.47619047619047616</v>
+        <f t="shared" si="2"/>
+        <v>-0.47619047619047616</v>
       </c>
       <c r="D23" s="10">
         <v>1.8436999999999999</v>
@@ -2799,18 +2815,18 @@
         <v>6.5582078962039532</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.87713634637295856</v>
       </c>
       <c r="H23" s="10">
         <v>53</v>
       </c>
       <c r="I23" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>20240126_00053</v>
+      </c>
+      <c r="J23" s="1">
         <f t="shared" si="10"/>
-        <v>20240126_00053</v>
-      </c>
-      <c r="J23" s="1">
-        <f t="shared" si="11"/>
         <v>2.4655048173156471E-2</v>
       </c>
     </row>
@@ -2819,11 +2835,11 @@
         <v>45317.477699884257</v>
       </c>
       <c r="B24" s="10">
-        <v>2.17</v>
+        <v>-2.17</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="1"/>
-        <v>0.46082949308755761</v>
+        <f t="shared" si="2"/>
+        <v>-0.46082949308755761</v>
       </c>
       <c r="D24" s="10">
         <v>1.8314999999999999</v>
@@ -2837,18 +2853,18 @@
         <v>7.176524251178364</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.86555260159513858</v>
       </c>
       <c r="H24" s="10">
         <v>56</v>
       </c>
       <c r="I24" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>20240126_00056</v>
+      </c>
+      <c r="J24" s="1">
         <f t="shared" si="10"/>
-        <v>20240126_00056</v>
-      </c>
-      <c r="J24" s="1">
-        <f t="shared" si="11"/>
         <v>2.4329445675091405E-2</v>
       </c>
     </row>
@@ -2857,11 +2873,11 @@
         <v>45317.541231481482</v>
       </c>
       <c r="B25" s="10">
-        <v>2.3199999999999998</v>
+        <v>-2.3199999999999998</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="1"/>
-        <v>0.43103448275862072</v>
+        <f t="shared" si="2"/>
+        <v>-0.43103448275862072</v>
       </c>
       <c r="D25" s="10">
         <v>1.8011999999999999</v>
@@ -2875,18 +2891,18 @@
         <v>8.7121788049262534</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.83678313710596275</v>
       </c>
       <c r="H25" s="10">
         <v>59</v>
       </c>
       <c r="I25" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>20240126_00059</v>
+      </c>
+      <c r="J25" s="1">
         <f t="shared" si="10"/>
-        <v>20240126_00059</v>
-      </c>
-      <c r="J25" s="1">
-        <f t="shared" si="11"/>
         <v>2.3520777175798657E-2</v>
       </c>
     </row>
@@ -2895,11 +2911,11 @@
         <v>45317.595966898145</v>
       </c>
       <c r="B26" s="10">
-        <v>2.4300000000000002</v>
+        <v>-2.4300000000000002</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="1"/>
-        <v>0.41152263374485593</v>
+        <f t="shared" si="2"/>
+        <v>-0.41152263374485593</v>
       </c>
       <c r="D26" s="10">
         <v>1.7742</v>
@@ -2913,28 +2929,28 @@
         <v>10.080583852820439</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>0.81114698063045954</v>
       </c>
       <c r="H26" s="10">
         <v>62</v>
       </c>
       <c r="I26" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>20240126_00062</v>
+      </c>
+      <c r="J26" s="1">
         <f t="shared" si="10"/>
-        <v>20240126_00062</v>
-      </c>
-      <c r="J26" s="1">
-        <f t="shared" si="11"/>
         <v>2.2800181483359574E-2</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D27" s="10"/>
@@ -2947,26 +2963,26 @@
         <v>#N/A</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-0.8734333459931638</v>
       </c>
       <c r="H27" s="10"/>
       <c r="I27" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>20240126_00000</v>
+      </c>
+      <c r="J27" s="1">
         <f t="shared" si="10"/>
-        <v>20240126_00000</v>
-      </c>
-      <c r="J27" s="1">
-        <f t="shared" si="11"/>
         <v>-2.4550962128693052E-2</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D28" s="10"/>
@@ -2979,26 +2995,26 @@
         <v>#N/A</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-0.8734333459931638</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>20240126_00000</v>
+      </c>
+      <c r="J28" s="1">
         <f t="shared" si="10"/>
-        <v>20240126_00000</v>
-      </c>
-      <c r="J28" s="1">
-        <f t="shared" si="11"/>
         <v>-2.4550962128693052E-2</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D29" s="10"/>
@@ -3011,16 +3027,16 @@
         <v>#N/A</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>-0.8734333459931638</v>
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>20240126_00000</v>
+      </c>
+      <c r="J29" s="1">
         <f t="shared" si="10"/>
-        <v>20240126_00000</v>
-      </c>
-      <c r="J29" s="1">
-        <f t="shared" si="11"/>
         <v>-2.4550962128693052E-2</v>
       </c>
     </row>

</xml_diff>